<commit_message>
update MV summary table with additional events
</commit_message>
<xml_diff>
--- a/MV_Summary_Table.xlsx
+++ b/MV_Summary_Table.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28410"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manga/Documents/papers/lusi_comment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Documents/PDX/Papers/Mazzini_Miller_Review_Comment/mv_triggering/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12780" windowHeight="16320" tabRatio="500"/>
+    <workbookView xWindow="13000" yWindow="460" windowWidth="14480" windowHeight="19360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,14 @@
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
+      <mx:ArchID Flags="4"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="74">
   <si>
     <t>MV</t>
   </si>
@@ -56,6 +56,9 @@
     <t>Niikappu</t>
   </si>
   <si>
+    <t>Salton Sea</t>
+  </si>
+  <si>
     <t>91 BC</t>
   </si>
   <si>
@@ -149,6 +152,9 @@
     <t>Caltanizetta, Italy</t>
   </si>
   <si>
+    <t>Rudolph and Manga (2012)</t>
+  </si>
+  <si>
     <t>Magnitude</t>
   </si>
   <si>
@@ -176,6 +182,9 @@
     <t>Tsunogai et al. (2012)</t>
   </si>
   <si>
+    <t>PGV (cm/s)</t>
+  </si>
+  <si>
     <t>Chigira and Tanaka (1997) with PGV from Manga et al. (2009)</t>
   </si>
   <si>
@@ -185,6 +194,9 @@
     <t>Manga and Brodsky (2006) with PGV from Manga et al. (2009)</t>
   </si>
   <si>
+    <t>Rudolph and Manga (2010) with PGV from Rudolph and Manga (2012)</t>
+  </si>
+  <si>
     <t>Torre, Italy</t>
   </si>
   <si>
@@ -195,13 +207,55 @@
   </si>
   <si>
     <t>Ospitaletto, Italy</t>
+  </si>
+  <si>
+    <t>S.Maria in Paganico, Italy</t>
+  </si>
+  <si>
+    <t>La Croce, Italy</t>
+  </si>
+  <si>
+    <t>Case tedeschi 2 bis, Italy</t>
+  </si>
+  <si>
+    <t>S. Maria in Paganico, Italy</t>
+  </si>
+  <si>
+    <t>Valle Corvone, Italy</t>
+  </si>
+  <si>
+    <t>Case Tedeschi 1, Italy</t>
+  </si>
+  <si>
+    <t>Case Tedeschi 3, Italy</t>
+  </si>
+  <si>
+    <t>Monteleone 1, Italy</t>
+  </si>
+  <si>
+    <t>Monteleone 2, Italy</t>
+  </si>
+  <si>
+    <t>Monteleone 3, Italy</t>
+  </si>
+  <si>
+    <t>Contrada S. Salvatore 1, Italy</t>
+  </si>
+  <si>
+    <t>Contrada S. Salvatore 2, Italy</t>
+  </si>
+  <si>
+    <t>Contrada S. Salvatore 3, Italy</t>
+  </si>
+  <si>
+    <t>Maestrelli et al. (2017)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -210,31 +264,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -254,76 +292,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="31">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -658,38 +636,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.5" customWidth="1"/>
+    <col min="3" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>28188</v>
       </c>
@@ -702,11 +683,11 @@
       <c r="D2">
         <v>92</v>
       </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>38347</v>
       </c>
@@ -719,11 +700,11 @@
       <c r="D3">
         <v>1030</v>
       </c>
-      <c r="E3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>37965</v>
       </c>
@@ -736,11 +717,11 @@
       <c r="D4">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>37965</v>
       </c>
@@ -753,11 +734,11 @@
       <c r="D5">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>41541</v>
       </c>
@@ -770,16 +751,19 @@
       <c r="D6">
         <v>383</v>
       </c>
-      <c r="E6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>3.4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>41049</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C7">
         <v>6.1</v>
@@ -787,16 +771,16 @@
       <c r="D7">
         <v>77</v>
       </c>
-      <c r="E7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>41049</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8">
         <v>6.1</v>
@@ -804,16 +788,16 @@
       <c r="D8">
         <v>63</v>
       </c>
-      <c r="E8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>41058</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9">
         <v>5.9</v>
@@ -821,16 +805,16 @@
       <c r="D9">
         <v>52</v>
       </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>41049</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C10">
         <v>6.1</v>
@@ -838,16 +822,16 @@
       <c r="D10">
         <v>63</v>
       </c>
-      <c r="E10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>41058</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C11">
         <v>5.9</v>
@@ -855,16 +839,16 @@
       <c r="D11">
         <v>52</v>
       </c>
-      <c r="E11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>41049</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12">
         <v>6.1</v>
@@ -872,16 +856,16 @@
       <c r="D12">
         <v>52</v>
       </c>
-      <c r="E12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>41049</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C13">
         <v>6.1</v>
@@ -889,16 +873,16 @@
       <c r="D13">
         <v>55</v>
       </c>
-      <c r="E13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>41058</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C14">
         <v>5.9</v>
@@ -906,11 +890,11 @@
       <c r="D14">
         <v>49</v>
       </c>
-      <c r="E14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>19057</v>
       </c>
@@ -923,11 +907,15 @@
       <c r="D15">
         <v>58</v>
       </c>
-      <c r="E15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <f>0.000428256*2500*100</f>
+        <v>107.06400000000001</v>
+      </c>
+      <c r="F15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>24974</v>
       </c>
@@ -940,11 +928,15 @@
       <c r="D16">
         <v>186</v>
       </c>
-      <c r="E16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <f>0.0000821983*2500*100</f>
+        <v>20.549574999999997</v>
+      </c>
+      <c r="F16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>30031</v>
       </c>
@@ -957,11 +949,15 @@
       <c r="D17">
         <v>25</v>
       </c>
-      <c r="E17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <f>0.000191308*2500*100</f>
+        <v>47.827000000000005</v>
+      </c>
+      <c r="F17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>33984</v>
       </c>
@@ -974,11 +970,15 @@
       <c r="D18">
         <v>153</v>
       </c>
-      <c r="E18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <f>0.000033396*2500*100</f>
+        <v>8.3490000000000002</v>
+      </c>
+      <c r="F18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>34696</v>
       </c>
@@ -991,11 +991,15 @@
       <c r="D19">
         <v>226</v>
       </c>
-      <c r="E19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <f>0.00003485*2500*100</f>
+        <v>8.7124999999999986</v>
+      </c>
+      <c r="F19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>37889</v>
       </c>
@@ -1008,420 +1012,764 @@
       <c r="D20">
         <v>145</v>
       </c>
-      <c r="E20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="E20">
+        <f>0.000127603*2500*100</f>
+        <v>31.900749999999999</v>
+      </c>
+      <c r="F20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>40272</v>
+      </c>
+      <c r="B21" t="s">
         <v>9</v>
       </c>
-      <c r="B21" t="s">
-        <v>33</v>
-      </c>
       <c r="C21">
+        <v>7.2</v>
+      </c>
+      <c r="D21">
+        <v>96.6</v>
+      </c>
+      <c r="E21">
+        <v>14.4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>41258</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D22">
+        <v>19</v>
+      </c>
+      <c r="E22">
+        <v>0.17</v>
+      </c>
+      <c r="F22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23">
         <v>5.7</v>
       </c>
-      <c r="D21">
+      <c r="D23">
         <v>15</v>
       </c>
-      <c r="E21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="F23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>10</v>
       </c>
-      <c r="C22">
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24">
         <v>5.7</v>
       </c>
-      <c r="D22">
+      <c r="D24">
         <v>14.5</v>
       </c>
-      <c r="E22" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="F24" t="s">
         <v>30</v>
       </c>
-      <c r="B23" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23">
-        <v>5.94</v>
-      </c>
-      <c r="D23">
-        <v>87</v>
-      </c>
-      <c r="E23" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24">
-        <v>5.09</v>
-      </c>
-      <c r="D24">
-        <v>12</v>
-      </c>
-      <c r="E24" t="s">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
-        <v>42062</v>
       </c>
       <c r="B25" t="s">
         <v>11</v>
       </c>
       <c r="C25">
+        <v>5.94</v>
+      </c>
+      <c r="D25">
+        <v>87</v>
+      </c>
+      <c r="F25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26">
+        <v>5.09</v>
+      </c>
+      <c r="D26">
+        <v>12</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <v>42062</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27">
         <v>7</v>
       </c>
-      <c r="D25">
+      <c r="D27">
         <v>340</v>
       </c>
-      <c r="E25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="F27" t="s">
         <v>13</v>
       </c>
-      <c r="C26">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28">
         <v>5.7</v>
       </c>
-      <c r="D26">
+      <c r="D28">
         <v>24</v>
       </c>
-      <c r="E26" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="F28" t="s">
         <v>15</v>
       </c>
-      <c r="C27">
-        <v>5.7</v>
-      </c>
-      <c r="D27">
-        <v>40</v>
-      </c>
-      <c r="E27" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
-        <v>775</v>
-      </c>
-      <c r="B28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28">
-        <v>6.9</v>
-      </c>
-      <c r="D28">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>45</v>
-      </c>
-      <c r="E28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
-        <v>775</v>
       </c>
       <c r="B29" t="s">
         <v>16</v>
       </c>
       <c r="C29">
+        <v>5.7</v>
+      </c>
+      <c r="D29">
+        <v>40</v>
+      </c>
+      <c r="F29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <v>775</v>
+      </c>
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30">
         <v>6.9</v>
       </c>
-      <c r="D29">
+      <c r="D30">
+        <v>45</v>
+      </c>
+      <c r="F30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
+        <v>775</v>
+      </c>
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31">
+        <v>6.9</v>
+      </c>
+      <c r="D31">
         <v>51</v>
       </c>
-      <c r="E29" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
-        <v>16769</v>
-      </c>
-      <c r="B30" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30">
-        <v>8.1</v>
-      </c>
-      <c r="D30">
-        <v>41</v>
-      </c>
-      <c r="E30" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
-        <v>16769</v>
-      </c>
-      <c r="B31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31">
-        <v>8.1</v>
-      </c>
-      <c r="D31">
-        <v>189</v>
-      </c>
-      <c r="E31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>16769</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C32">
         <v>8.1</v>
       </c>
       <c r="D32">
+        <v>41</v>
+      </c>
+      <c r="F32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <v>16769</v>
+      </c>
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33">
+        <v>8.1</v>
+      </c>
+      <c r="D33">
+        <v>189</v>
+      </c>
+      <c r="F33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <v>16769</v>
+      </c>
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34">
+        <v>8.1</v>
+      </c>
+      <c r="D34">
         <v>155</v>
       </c>
-      <c r="E32" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="3">
+      <c r="F34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
         <v>12934</v>
       </c>
-      <c r="B33" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33">
+      <c r="B35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35">
         <v>7.7</v>
       </c>
-      <c r="D33">
+      <c r="D35">
         <v>61</v>
       </c>
-      <c r="E33" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="F35" t="s">
         <v>23</v>
       </c>
-      <c r="C34">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36">
         <v>8.1999999999999993</v>
       </c>
-      <c r="D34">
+      <c r="D36">
         <v>141</v>
       </c>
-      <c r="E34" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>45</v>
-      </c>
-      <c r="B35" t="s">
-        <v>24</v>
-      </c>
-      <c r="C35">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="D35">
+      <c r="F36" t="s">
         <v>15</v>
       </c>
-      <c r="E35" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="2">
-        <v>21158</v>
-      </c>
-      <c r="B36" t="s">
-        <v>25</v>
-      </c>
-      <c r="C36">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="D36">
-        <v>75</v>
-      </c>
-      <c r="E36" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="2">
-        <v>38883</v>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>47</v>
       </c>
       <c r="B37" t="s">
         <v>25</v>
       </c>
       <c r="C37">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D37">
+        <v>15</v>
+      </c>
+      <c r="F37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>21158</v>
+      </c>
+      <c r="B38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D38">
+        <v>75</v>
+      </c>
+      <c r="F38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>38883</v>
+      </c>
+      <c r="B39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39">
         <v>5.8</v>
       </c>
-      <c r="D37">
+      <c r="D39">
         <v>90</v>
       </c>
-      <c r="E37" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
+      <c r="F39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
         <v>36917</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40">
+        <v>7.7</v>
+      </c>
+      <c r="D40">
+        <v>482</v>
+      </c>
+      <c r="F40" t="s">
         <v>28</v>
       </c>
-      <c r="C38">
-        <v>7.7</v>
-      </c>
-      <c r="D38">
-        <v>482</v>
-      </c>
-      <c r="E38" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="2">
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
         <v>5763</v>
       </c>
-      <c r="B39" t="s">
-        <v>32</v>
-      </c>
-      <c r="C39">
+      <c r="B41" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41">
         <v>5</v>
       </c>
-      <c r="D39">
+      <c r="D41">
         <v>21</v>
       </c>
-      <c r="E39" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="F41" t="s">
         <v>35</v>
       </c>
-      <c r="B40" t="s">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>36</v>
-      </c>
-      <c r="C40">
-        <v>5</v>
-      </c>
-      <c r="D40">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E40" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="2">
-        <v>33220</v>
-      </c>
-      <c r="B41" t="s">
-        <v>37</v>
-      </c>
-      <c r="C41">
-        <v>5.7</v>
-      </c>
-      <c r="D41">
-        <v>39</v>
-      </c>
-      <c r="E41" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="2">
-        <v>28767</v>
       </c>
       <c r="B42" t="s">
         <v>37</v>
       </c>
       <c r="C42">
+        <v>5</v>
+      </c>
+      <c r="D42">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F42" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
+        <v>33220</v>
+      </c>
+      <c r="B43" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43">
+        <v>5.7</v>
+      </c>
+      <c r="D43">
+        <v>39</v>
+      </c>
+      <c r="F43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
+        <v>28767</v>
+      </c>
+      <c r="B44" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44">
         <v>5.2</v>
       </c>
-      <c r="D42">
+      <c r="D44">
         <v>34</v>
       </c>
-      <c r="E42" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>38</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="F44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>39</v>
       </c>
-      <c r="C43">
+      <c r="B45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45">
         <v>5.9</v>
       </c>
-      <c r="D43">
+      <c r="D45">
         <v>56</v>
       </c>
-      <c r="E43" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="2">
+      <c r="F45" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
         <v>38235</v>
       </c>
-      <c r="B44" t="s">
-        <v>47</v>
-      </c>
-      <c r="C44">
+      <c r="B46" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46">
         <v>7.4</v>
       </c>
-      <c r="D44">
+      <c r="D46">
         <v>80</v>
       </c>
-      <c r="E44" t="s">
-        <v>48</v>
+      <c r="F46" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
+        <v>42606</v>
+      </c>
+      <c r="B47" t="s">
+        <v>60</v>
+      </c>
+      <c r="C47">
+        <v>6</v>
+      </c>
+      <c r="D47">
+        <v>48.25</v>
+      </c>
+      <c r="E47">
+        <v>6.3</v>
+      </c>
+      <c r="F47" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="3">
+        <v>42607</v>
+      </c>
+      <c r="B48" t="s">
+        <v>61</v>
+      </c>
+      <c r="C48">
+        <v>6</v>
+      </c>
+      <c r="D48">
+        <v>44.94</v>
+      </c>
+      <c r="E48">
+        <v>7.34</v>
+      </c>
+      <c r="F48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="3">
+        <v>42608</v>
+      </c>
+      <c r="B49" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49">
+        <v>6</v>
+      </c>
+      <c r="D49">
+        <v>44.7</v>
+      </c>
+      <c r="E49">
+        <v>7.34</v>
+      </c>
+      <c r="F49" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="3">
+        <v>42673</v>
+      </c>
+      <c r="B50" t="s">
+        <v>63</v>
+      </c>
+      <c r="C50">
+        <v>6.5</v>
+      </c>
+      <c r="D50">
+        <v>43.44</v>
+      </c>
+      <c r="E50">
+        <v>5.62</v>
+      </c>
+      <c r="F50" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="3">
+        <v>42674</v>
+      </c>
+      <c r="B51" t="s">
+        <v>64</v>
+      </c>
+      <c r="C51">
+        <v>6.5</v>
+      </c>
+      <c r="D51">
+        <v>40.93</v>
+      </c>
+      <c r="E51">
+        <v>6.41</v>
+      </c>
+      <c r="F51" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="3">
+        <v>42675</v>
+      </c>
+      <c r="B52" t="s">
+        <v>61</v>
+      </c>
+      <c r="C52">
+        <v>6.5</v>
+      </c>
+      <c r="D52">
+        <v>40.770000000000003</v>
+      </c>
+      <c r="E52">
+        <v>6.36</v>
+      </c>
+      <c r="F52" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="3">
+        <v>42676</v>
+      </c>
+      <c r="B53" t="s">
+        <v>65</v>
+      </c>
+      <c r="C53">
+        <v>6.5</v>
+      </c>
+      <c r="D53">
+        <v>40.68</v>
+      </c>
+      <c r="E53">
+        <v>6.26</v>
+      </c>
+      <c r="F53" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="3">
+        <v>42677</v>
+      </c>
+      <c r="B54" t="s">
+        <v>66</v>
+      </c>
+      <c r="C54">
+        <v>6.5</v>
+      </c>
+      <c r="D54">
+        <v>40.67</v>
+      </c>
+      <c r="E54">
+        <v>6.22</v>
+      </c>
+      <c r="F54" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="3">
+        <v>42678</v>
+      </c>
+      <c r="B55" t="s">
+        <v>67</v>
+      </c>
+      <c r="C55">
+        <v>6.5</v>
+      </c>
+      <c r="D55">
+        <v>40.97</v>
+      </c>
+      <c r="E55">
+        <v>6.23</v>
+      </c>
+      <c r="F55" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="3">
+        <v>42679</v>
+      </c>
+      <c r="B56" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56">
+        <v>6.5</v>
+      </c>
+      <c r="D56">
+        <v>40.96</v>
+      </c>
+      <c r="E56">
+        <v>6.2</v>
+      </c>
+      <c r="F56" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="3">
+        <v>42680</v>
+      </c>
+      <c r="B57" t="s">
+        <v>69</v>
+      </c>
+      <c r="C57">
+        <v>6.5</v>
+      </c>
+      <c r="D57">
+        <v>40.909999999999997</v>
+      </c>
+      <c r="E57">
+        <v>6.2</v>
+      </c>
+      <c r="F57" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="3">
+        <v>42681</v>
+      </c>
+      <c r="B58" t="s">
+        <v>70</v>
+      </c>
+      <c r="C58">
+        <v>6.5</v>
+      </c>
+      <c r="D58">
+        <v>37.729999999999997</v>
+      </c>
+      <c r="E58">
+        <v>8.76</v>
+      </c>
+      <c r="F58" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="3">
+        <v>42682</v>
+      </c>
+      <c r="B59" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59">
+        <v>6.5</v>
+      </c>
+      <c r="D59">
+        <v>37.659999999999997</v>
+      </c>
+      <c r="E59">
+        <v>9.01</v>
+      </c>
+      <c r="F59" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="3">
+        <v>42683</v>
+      </c>
+      <c r="B60" t="s">
+        <v>72</v>
+      </c>
+      <c r="C60">
+        <v>6.5</v>
+      </c>
+      <c r="D60">
+        <v>37.72</v>
+      </c>
+      <c r="E60">
+        <v>8.9700000000000006</v>
+      </c>
+      <c r="F60" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="3">
+        <v>42753</v>
+      </c>
+      <c r="B61" t="s">
+        <v>60</v>
+      </c>
+      <c r="C61">
+        <v>5.5</v>
+      </c>
+      <c r="D61">
+        <v>63.81</v>
+      </c>
+      <c r="E61">
+        <v>1.28</v>
+      </c>
+      <c r="F61" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>

</xml_diff>

<commit_message>
add 2024 bledug kuwu
</commit_message>
<xml_diff>
--- a/MV_Summary_Table.xlsx
+++ b/MV_Summary_Table.xlsx
@@ -1,23 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Documents/PDX/Papers/Mazzini_Miller_Review_Comment/mv_triggering/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Desktop/mv_triggering/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F70E34E-6CE1-1945-983B-47493077E88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13000" yWindow="460" windowWidth="14480" windowHeight="19360" tabRatio="500"/>
+    <workbookView xWindow="2640" yWindow="860" windowWidth="29720" windowHeight="20240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="4"/>
@@ -27,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="76">
   <si>
     <t>MV</t>
   </si>
@@ -249,13 +261,19 @@
   </si>
   <si>
     <t>Maestrelli et al. (2017)</t>
+  </si>
+  <si>
+    <t>Tingay, Pers. Comm.</t>
+  </si>
+  <si>
+    <t>Bledug Kuwu, Cangkring, East Java</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -273,6 +291,13 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -295,11 +320,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -309,6 +335,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -635,17 +664,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A44" zoomScale="178" zoomScaleNormal="178" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" customWidth="1"/>
     <col min="3" max="5" width="16.6640625" customWidth="1"/>
     <col min="6" max="6" width="19.5" customWidth="1"/>
   </cols>
@@ -1768,6 +1797,23 @@
         <v>73</v>
       </c>
     </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="3">
+        <v>45373</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C62">
+        <v>6.4</v>
+      </c>
+      <c r="D62">
+        <v>195</v>
+      </c>
+      <c r="F62" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>